<commit_message>
tidy endpoint mapping and persistence code
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -438,13 +438,13 @@
     <t xml:space="preserve">If the file is split into parts</t>
   </si>
   <si>
-    <t xml:space="preserve">recordingLength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hearing File Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File length in minutes</t>
+    <t xml:space="preserve">fileSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearing File Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File size in MBs</t>
   </si>
   <si>
     <t xml:space="preserve">FixedLists</t>
@@ -6380,8 +6380,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10118,8 +10118,8 @@
   </sheetPr>
   <dimension ref="A1:IU18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
use valid document url as ccd-date-store checks it
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="302">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -293,25 +293,16 @@
     <t xml:space="preserve">FixedList</t>
   </si>
   <si>
-    <t xml:space="preserve">caseFileCaseID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filename prefix that identifies the CaseID</t>
+    <t xml:space="preserve">hearingRoomRef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearing Room Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical or Virtual room</t>
   </si>
   <si>
     <t xml:space="preserve">Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hearingRoomRef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hearing Room Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physical or Virtual room</t>
   </si>
   <si>
     <t xml:space="preserve">recordingDateTime</t>
@@ -2346,7 +2337,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -2373,31 +2364,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>175</v>
-      </c>
       <c r="J2" s="17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -2424,28 +2415,28 @@
         <v>19</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F3" s="90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G3" s="89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H3" s="89" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I3" s="89" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J3" s="89" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K3" s="89" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2466,8 +2457,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2489,7 +2480,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="12" t="s">
@@ -2520,31 +2511,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="K2" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="L2" s="16" t="s">
         <v>220</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2558,31 +2549,31 @@
         <v>49</v>
       </c>
       <c r="D3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="H3" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>229</v>
-      </c>
       <c r="L3" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M3" s="61"/>
       <c r="N3" s="61"/>
@@ -2597,10 +2588,10 @@
       </c>
       <c r="D4" s="62"/>
       <c r="E4" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F4" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
         <v>1</v>
@@ -2625,10 +2616,10 @@
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
         <v>1</v>
@@ -2637,7 +2628,7 @@
         <v>75</v>
       </c>
       <c r="I5" s="62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="62"/>
@@ -2653,10 +2644,10 @@
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F6" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
         <v>1</v>
@@ -2665,7 +2656,7 @@
         <v>79</v>
       </c>
       <c r="I6" s="62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J6" s="62"/>
       <c r="K6" s="62"/>
@@ -2681,19 +2672,19 @@
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F7" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I7" s="62" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="62"/>
@@ -2709,19 +2700,19 @@
       </c>
       <c r="D8" s="62"/>
       <c r="E8" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F8" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="62" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="62"/>
@@ -2737,19 +2728,19 @@
       </c>
       <c r="D9" s="62"/>
       <c r="E9" s="91" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F9" s="92" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I9" s="62" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="62"/>
@@ -2765,57 +2756,30 @@
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="91" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="92" t="s">
-        <v>231</v>
+        <v>94</v>
       </c>
       <c r="G10" s="62" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="62" t="n">
         <v>1</v>
-      </c>
-      <c r="H10" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="62" t="n">
-        <v>7</v>
       </c>
       <c r="J10" s="62"/>
       <c r="K10" s="62"/>
       <c r="L10" s="62"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="49" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="91" t="s">
-        <v>232</v>
-      </c>
-      <c r="F11" s="92" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="62" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86"/>
-      <c r="C12" s="28"/>
-      <c r="H12" s="87"/>
-    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="86"/>
+      <c r="C11" s="28"/>
+      <c r="H11" s="87"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2856,7 +2820,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="94" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>8</v>
@@ -2891,22 +2855,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="101" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="101" t="s">
+        <v>232</v>
+      </c>
+      <c r="G2" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" s="102" t="s">
+        <v>233</v>
+      </c>
+      <c r="I2" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="J2" s="101" t="s">
         <v>235</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>208</v>
-      </c>
-      <c r="H2" s="102" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" s="103" t="s">
-        <v>237</v>
-      </c>
-      <c r="J2" s="101" t="s">
-        <v>238</v>
       </c>
       <c r="K2" s="102"/>
       <c r="L2" s="104"/>
@@ -2929,22 +2893,22 @@
         <v>50</v>
       </c>
       <c r="F3" s="106" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="106" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="107" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="107" t="s">
         <v>239</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="K3" s="107" t="s">
         <v>240</v>
-      </c>
-      <c r="H3" s="107" t="s">
-        <v>241</v>
-      </c>
-      <c r="I3" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="107" t="s">
-        <v>242</v>
-      </c>
-      <c r="K3" s="107" t="s">
-        <v>243</v>
       </c>
       <c r="L3" s="107"/>
       <c r="M3" s="108"/>
@@ -3036,10 +3000,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3059,7 +3023,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B1" s="110" t="s">
         <v>8</v>
@@ -3088,25 +3052,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3120,25 +3084,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>64</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3150,11 +3114,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="74" t="n">
@@ -3172,11 +3136,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="52" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" s="50"/>
       <c r="H5" s="74" t="n">
@@ -3194,11 +3158,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G6" s="50"/>
       <c r="H6" s="74" t="n">
@@ -3216,11 +3180,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="74" t="n">
@@ -3238,62 +3202,43 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="74" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="50"/>
     </row>
-    <row r="9" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="50"/>
+        <v>79</v>
+      </c>
+      <c r="E9" s="62"/>
+      <c r="F9" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="62"/>
       <c r="H9" s="74" t="n">
-        <v>6</v>
-      </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-    </row>
-    <row r="10" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+    </row>
+    <row r="10" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="65"/>
     </row>
     <row r="11" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="65"/>
@@ -3325,10 +3270,8 @@
     <row r="20" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="65"/>
     </row>
-    <row r="21" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="65"/>
-    </row>
-    <row r="22" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -3345,10 +3288,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3368,7 +3311,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3396,22 +3339,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="116" t="s">
         <v>249</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="116" t="s">
-        <v>252</v>
       </c>
       <c r="J2" s="117"/>
       <c r="K2" s="118"/>
@@ -3429,10 +3372,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="89" t="s">
         <v>64</v>
@@ -3441,10 +3384,10 @@
         <v>50</v>
       </c>
       <c r="H3" s="89" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I3" s="120" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J3" s="121"/>
       <c r="K3" s="122"/>
@@ -3460,11 +3403,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -3482,11 +3425,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="52" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" s="74" t="n">
         <v>2</v>
@@ -3504,11 +3447,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -3526,11 +3469,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -3548,20 +3491,20 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="52"/>
+        <v>85</v>
+      </c>
+      <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G8" s="74" t="n">
-        <v>5</v>
-      </c>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-    </row>
-    <row r="9" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" s="123" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3570,40 +3513,23 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="52" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G9" s="74" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
     </row>
-    <row r="10" s="123" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="74" t="n">
-        <v>7</v>
-      </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="86"/>
+      <c r="C10" s="28"/>
+      <c r="G10" s="124"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="86"/>
@@ -3612,7 +3538,6 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="86"/>
-      <c r="C12" s="28"/>
       <c r="G12" s="124"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3623,10 +3548,7 @@
       <c r="A14" s="86"/>
       <c r="G14" s="124"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="86"/>
-      <c r="G15" s="124"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -3665,7 +3587,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="125" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
         <v>8</v>
@@ -3686,16 +3608,16 @@
       <c r="A2" s="88"/>
       <c r="B2" s="88"/>
       <c r="C2" s="127" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D2" s="127" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E2" s="127" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F2" s="88" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G2" s="88"/>
       <c r="H2" s="88"/>
@@ -3712,7 +3634,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="129" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="128" t="s">
         <v>64</v>
@@ -3721,13 +3643,13 @@
         <v>50</v>
       </c>
       <c r="G3" s="128" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H3" s="128" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I3" s="128" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3746,10 +3668,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3768,7 +3690,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="131" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B1" s="132" t="s">
         <v>8</v>
@@ -3797,25 +3719,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3829,25 +3751,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="89" t="s">
         <v>64</v>
       </c>
       <c r="G3" s="89" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H3" s="89" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="89" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J3" s="89" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3859,11 +3781,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="74" t="n">
@@ -3881,11 +3803,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="52" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="74" t="n">
@@ -3903,11 +3825,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="74" t="n">
@@ -3925,11 +3847,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="74" t="n">
@@ -3938,7 +3860,7 @@
       <c r="I7" s="50"/>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3947,18 +3869,18 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="52"/>
+        <v>85</v>
+      </c>
+      <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="74"/>
+        <v>86</v>
+      </c>
+      <c r="G8" s="25"/>
       <c r="H8" s="74" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
+        <v>6</v>
+      </c>
+      <c r="I8" s="135"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
@@ -3969,15 +3891,15 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="52" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="74" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I9" s="135"/>
       <c r="J9" s="62"/>
@@ -3995,37 +3917,16 @@
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="52" t="s">
-        <v>83</v>
+        <v>257</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="74" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10" s="135"/>
       <c r="J10" s="62"/>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="52" t="s">
-        <v>260</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="74" t="n">
-        <v>8</v>
-      </c>
-      <c r="I11" s="135"/>
-      <c r="J11" s="62"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -4042,10 +3943,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4064,7 +3965,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4092,22 +3993,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4121,10 +4022,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="89" t="s">
         <v>64</v>
@@ -4133,10 +4034,10 @@
         <v>50</v>
       </c>
       <c r="H3" s="89" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I3" s="89" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J3" s="122"/>
       <c r="K3" s="122"/>
@@ -4152,11 +4053,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -4174,11 +4075,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="52" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" s="74" t="n">
         <v>2</v>
@@ -4196,11 +4097,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -4218,11 +4119,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -4240,14 +4141,14 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G8" s="74" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" s="50"/>
       <c r="I8" s="50"/>
@@ -4262,14 +4163,14 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="52" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G9" s="74" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
@@ -4288,36 +4189,21 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52" t="s">
-        <v>83</v>
+        <v>257</v>
       </c>
       <c r="G10" s="74" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="50"/>
       <c r="I10" s="50"/>
       <c r="J10" s="50"/>
     </row>
-    <row r="11" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52" t="s">
-        <v>260</v>
-      </c>
-      <c r="G11" s="74" t="n">
-        <v>8</v>
-      </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="86"/>
@@ -4340,13 +4226,7 @@
       <c r="D14" s="136"/>
       <c r="F14" s="136"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="136"/>
-      <c r="F15" s="136"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -4384,7 +4264,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4407,13 +4287,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4424,16 +4304,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" s="79" t="s">
         <v>266</v>
-      </c>
-      <c r="D3" s="79" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="79" t="s">
-        <v>268</v>
-      </c>
-      <c r="F3" s="79" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4442,7 +4322,7 @@
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="137" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D4" s="137" t="s">
         <v>23</v>
@@ -4494,7 +4374,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4516,16 +4396,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4715,7 +4595,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4736,13 +4616,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4756,10 +4636,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4771,10 +4651,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -4796,10 +4676,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="53"/>
@@ -4833,8 +4713,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4851,7 +4731,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="140" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4877,16 +4757,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G2" s="127"/>
       <c r="H2" s="127"/>
@@ -4905,13 +4785,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="143" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="143" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F3" s="142" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G3" s="88"/>
       <c r="H3" s="88"/>
@@ -4931,10 +4811,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -4946,7 +4826,7 @@
       <c r="N4" s="53"/>
       <c r="O4" s="53"/>
     </row>
-    <row r="5" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
@@ -4958,10 +4838,10 @@
         <v>75</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4976,10 +4856,10 @@
         <v>79</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4994,10 +4874,10 @@
         <v>82</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5012,13 +4892,13 @@
         <v>85</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5027,16 +4907,16 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5045,13 +4925,13 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5063,13 +4943,13 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5081,13 +4961,13 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5098,17 +4978,17 @@
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>96</v>
+      <c r="D13" s="25" t="s">
+        <v>97</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5116,17 +4996,26 @@
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>100</v>
+      <c r="D14" s="52" t="s">
+        <v>71</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5135,25 +5024,16 @@
         <v>38</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>278</v>
-      </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="53"/>
-    </row>
-    <row r="16" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5162,13 +5042,13 @@
         <v>38</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5180,13 +5060,13 @@
         <v>38</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5198,16 +5078,16 @@
         <v>38</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5216,13 +5096,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5234,16 +5114,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="n">
         <v>44197</v>
       </c>
@@ -5252,13 +5132,13 @@
         <v>38</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5270,13 +5150,13 @@
         <v>38</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5287,52 +5167,18 @@
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="52" t="s">
-        <v>94</v>
+      <c r="D23" s="25" t="s">
+        <v>97</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B24" s="115"/>
-      <c r="C24" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>280</v>
-      </c>
-      <c r="F24" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="49" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B25" s="115"/>
-      <c r="C25" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>280</v>
-      </c>
-      <c r="F25" s="51" t="s">
-        <v>278</v>
-      </c>
-    </row>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5383,7 +5229,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5405,16 +5251,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -5433,13 +5279,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="144" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5451,13 +5297,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5469,13 +5315,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5487,13 +5333,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5505,13 +5351,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5523,13 +5369,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5541,13 +5387,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5559,13 +5405,13 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5577,13 +5423,13 @@
         <v>38</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5626,7 +5472,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="146" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B1" s="147" t="s">
         <v>8</v>
@@ -5648,16 +5494,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="151" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G2" s="152"/>
       <c r="H2" s="152"/>
@@ -5676,13 +5522,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="144" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F3" s="153" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5697,10 +5543,10 @@
         <v>52</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -5726,10 +5572,10 @@
         <v>52</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
@@ -5780,7 +5626,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5799,19 +5645,19 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,16 +5671,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5846,16 +5692,16 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5867,16 +5713,16 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5888,16 +5734,16 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5909,16 +5755,16 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5930,16 +5776,16 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5951,16 +5797,16 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G9" s="51" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5997,7 +5843,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="154" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B1" s="155"/>
       <c r="C1" s="155"/>
@@ -6005,44 +5851,44 @@
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="157" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="157" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" s="157" t="s">
         <v>293</v>
-      </c>
-      <c r="B2" s="157" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="157" t="s">
-        <v>295</v>
-      </c>
-      <c r="D2" s="157" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="158" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" s="158" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="158" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="158" t="s">
         <v>297</v>
-      </c>
-      <c r="B3" s="158" t="s">
-        <v>298</v>
-      </c>
-      <c r="C3" s="158" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="158" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="159" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="160" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="160" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>301</v>
-      </c>
-      <c r="B4" s="160" t="s">
-        <v>302</v>
-      </c>
-      <c r="C4" s="160" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,10 +6224,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6845,14 +6691,12 @@
       <c r="D6" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="62"/>
+      <c r="G6" s="62" t="s">
         <v>81</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>78</v>
       </c>
       <c r="H6" s="62"/>
       <c r="I6" s="62"/>
@@ -7009,12 +6853,14 @@
       <c r="D7" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="62" t="s">
         <v>84</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>78</v>
       </c>
       <c r="H7" s="62"/>
       <c r="I7" s="62"/>
@@ -7174,9 +7020,7 @@
       <c r="E8" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>87</v>
-      </c>
+      <c r="F8" s="62"/>
       <c r="G8" s="51" t="s">
         <v>78</v>
       </c>
@@ -7332,11 +7176,11 @@
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="52" t="s">
         <v>88</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>89</v>
       </c>
       <c r="F9" s="62"/>
       <c r="G9" s="51" t="s">
@@ -7495,10 +7339,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="52" t="s">
         <v>90</v>
-      </c>
-      <c r="E10" s="52" t="s">
-        <v>91</v>
       </c>
       <c r="F10" s="62"/>
       <c r="G10" s="51" t="s">
@@ -7657,10 +7501,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="52" t="s">
         <v>92</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>93</v>
       </c>
       <c r="F11" s="62"/>
       <c r="G11" s="51" t="s">
@@ -7818,17 +7662,19 @@
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="F12" s="50"/>
+      <c r="G12" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="52" t="s">
+        <v>96</v>
+      </c>
       <c r="I12" s="62"/>
       <c r="J12" s="51" t="s">
         <v>41</v>
@@ -7980,19 +7826,17 @@
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="52" t="s">
+      <c r="D13" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="50"/>
+      <c r="E13" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="62"/>
       <c r="G13" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>99</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H13" s="62"/>
       <c r="I13" s="62"/>
       <c r="J13" s="51" t="s">
         <v>41</v>
@@ -8137,30 +7981,124 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
+      <c r="A14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="53"/>
+      <c r="AC14" s="53"/>
+      <c r="AD14" s="53"/>
+      <c r="AE14" s="53"/>
+      <c r="AF14" s="53"/>
+      <c r="AG14" s="53"/>
+      <c r="AH14" s="53"/>
+      <c r="AI14" s="53"/>
+      <c r="AJ14" s="53"/>
+      <c r="AK14" s="53"/>
+      <c r="AL14" s="53"/>
+      <c r="AM14" s="53"/>
+      <c r="AN14" s="53"/>
+      <c r="AO14" s="53"/>
+      <c r="AP14" s="53"/>
+      <c r="AQ14" s="53"/>
+      <c r="AR14" s="53"/>
+      <c r="AS14" s="53"/>
+      <c r="AT14" s="53"/>
+      <c r="AU14" s="53"/>
+      <c r="AV14" s="53"/>
+      <c r="AW14" s="53"/>
+      <c r="AX14" s="53"/>
+      <c r="AY14" s="53"/>
+      <c r="AZ14" s="53"/>
+      <c r="BA14" s="53"/>
+      <c r="BB14" s="53"/>
+      <c r="BC14" s="53"/>
+      <c r="BD14" s="53"/>
+      <c r="BE14" s="53"/>
+      <c r="BF14" s="53"/>
+      <c r="BG14" s="53"/>
+      <c r="BH14" s="53"/>
+      <c r="BI14" s="53"/>
+      <c r="BJ14" s="53"/>
+      <c r="BK14" s="53"/>
+      <c r="BL14" s="53"/>
+      <c r="BM14" s="53"/>
+      <c r="BN14" s="53"/>
+      <c r="BO14" s="53"/>
+      <c r="BP14" s="53"/>
+      <c r="BQ14" s="53"/>
+      <c r="BR14" s="53"/>
+      <c r="BS14" s="53"/>
+      <c r="BT14" s="53"/>
+      <c r="BU14" s="53"/>
+      <c r="BV14" s="53"/>
+      <c r="BW14" s="53"/>
+      <c r="BX14" s="53"/>
+      <c r="BY14" s="53"/>
+      <c r="BZ14" s="53"/>
+      <c r="CA14" s="53"/>
+      <c r="CB14" s="53"/>
+      <c r="CC14" s="53"/>
+      <c r="CD14" s="53"/>
+      <c r="CE14" s="53"/>
+      <c r="CF14" s="53"/>
+      <c r="CG14" s="53"/>
+      <c r="CH14" s="53"/>
+      <c r="CI14" s="53"/>
+      <c r="CJ14" s="53"/>
+      <c r="CK14" s="53"/>
+      <c r="CL14" s="53"/>
+      <c r="CM14" s="53"/>
+      <c r="CN14" s="53"/>
+      <c r="CO14" s="53"/>
+      <c r="CP14" s="53"/>
+      <c r="CQ14" s="53"/>
+      <c r="CR14" s="53"/>
+      <c r="CS14" s="53"/>
+      <c r="CT14" s="53"/>
+      <c r="CU14" s="53"/>
+      <c r="CV14" s="53"/>
+      <c r="CW14" s="53"/>
+      <c r="CX14" s="53"/>
+      <c r="CY14" s="53"/>
+      <c r="CZ14" s="53"/>
+      <c r="DA14" s="53"/>
+      <c r="DB14" s="53"/>
+      <c r="DC14" s="53"/>
+      <c r="DD14" s="53"/>
+      <c r="DE14" s="53"/>
+      <c r="DF14" s="53"/>
+      <c r="DG14" s="53"/>
+      <c r="DH14" s="53"/>
+      <c r="DI14" s="53"/>
+      <c r="DJ14" s="53"/>
+      <c r="DK14" s="53"/>
+      <c r="DL14" s="53"/>
+      <c r="DM14" s="53"/>
+      <c r="DN14" s="53"/>
+      <c r="DO14" s="53"/>
       <c r="AHE14" s="0"/>
       <c r="AHF14" s="0"/>
       <c r="AHG14" s="0"/>
@@ -8298,125 +8236,7 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="53"/>
-      <c r="P15" s="53"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="53"/>
-      <c r="T15" s="53"/>
-      <c r="U15" s="53"/>
-      <c r="V15" s="53"/>
-      <c r="W15" s="53"/>
-      <c r="X15" s="53"/>
-      <c r="Y15" s="53"/>
-      <c r="Z15" s="53"/>
-      <c r="AA15" s="53"/>
-      <c r="AB15" s="53"/>
-      <c r="AC15" s="53"/>
-      <c r="AD15" s="53"/>
-      <c r="AE15" s="53"/>
-      <c r="AF15" s="53"/>
-      <c r="AG15" s="53"/>
-      <c r="AH15" s="53"/>
-      <c r="AI15" s="53"/>
-      <c r="AJ15" s="53"/>
-      <c r="AK15" s="53"/>
-      <c r="AL15" s="53"/>
-      <c r="AM15" s="53"/>
-      <c r="AN15" s="53"/>
-      <c r="AO15" s="53"/>
-      <c r="AP15" s="53"/>
-      <c r="AQ15" s="53"/>
-      <c r="AR15" s="53"/>
-      <c r="AS15" s="53"/>
-      <c r="AT15" s="53"/>
-      <c r="AU15" s="53"/>
-      <c r="AV15" s="53"/>
-      <c r="AW15" s="53"/>
-      <c r="AX15" s="53"/>
-      <c r="AY15" s="53"/>
-      <c r="AZ15" s="53"/>
-      <c r="BA15" s="53"/>
-      <c r="BB15" s="53"/>
-      <c r="BC15" s="53"/>
-      <c r="BD15" s="53"/>
-      <c r="BE15" s="53"/>
-      <c r="BF15" s="53"/>
-      <c r="BG15" s="53"/>
-      <c r="BH15" s="53"/>
-      <c r="BI15" s="53"/>
-      <c r="BJ15" s="53"/>
-      <c r="BK15" s="53"/>
-      <c r="BL15" s="53"/>
-      <c r="BM15" s="53"/>
-      <c r="BN15" s="53"/>
-      <c r="BO15" s="53"/>
-      <c r="BP15" s="53"/>
-      <c r="BQ15" s="53"/>
-      <c r="BR15" s="53"/>
-      <c r="BS15" s="53"/>
-      <c r="BT15" s="53"/>
-      <c r="BU15" s="53"/>
-      <c r="BV15" s="53"/>
-      <c r="BW15" s="53"/>
-      <c r="BX15" s="53"/>
-      <c r="BY15" s="53"/>
-      <c r="BZ15" s="53"/>
-      <c r="CA15" s="53"/>
-      <c r="CB15" s="53"/>
-      <c r="CC15" s="53"/>
-      <c r="CD15" s="53"/>
-      <c r="CE15" s="53"/>
-      <c r="CF15" s="53"/>
-      <c r="CG15" s="53"/>
-      <c r="CH15" s="53"/>
-      <c r="CI15" s="53"/>
-      <c r="CJ15" s="53"/>
-      <c r="CK15" s="53"/>
-      <c r="CL15" s="53"/>
-      <c r="CM15" s="53"/>
-      <c r="CN15" s="53"/>
-      <c r="CO15" s="53"/>
-      <c r="CP15" s="53"/>
-      <c r="CQ15" s="53"/>
-      <c r="CR15" s="53"/>
-      <c r="CS15" s="53"/>
-      <c r="CT15" s="53"/>
-      <c r="CU15" s="53"/>
-      <c r="CV15" s="53"/>
-      <c r="CW15" s="53"/>
-      <c r="CX15" s="53"/>
-      <c r="CY15" s="53"/>
-      <c r="CZ15" s="53"/>
-      <c r="DA15" s="53"/>
-      <c r="DB15" s="53"/>
-      <c r="DC15" s="53"/>
-      <c r="DD15" s="53"/>
-      <c r="DE15" s="53"/>
-      <c r="DF15" s="53"/>
-      <c r="DG15" s="53"/>
-      <c r="DH15" s="53"/>
-      <c r="DI15" s="53"/>
-      <c r="DJ15" s="53"/>
-      <c r="DK15" s="53"/>
-      <c r="DL15" s="53"/>
-      <c r="DM15" s="53"/>
-      <c r="DN15" s="53"/>
-      <c r="DO15" s="53"/>
+    <row r="15" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AHE15" s="0"/>
       <c r="AHF15" s="0"/>
       <c r="AHG15" s="0"/>
@@ -8555,6 +8375,10 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="66"/>
       <c r="AHE16" s="0"/>
       <c r="AHF16" s="0"/>
       <c r="AHG16" s="0"/>
@@ -8694,9 +8518,8 @@
     </row>
     <row r="17" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="E17" s="65"/>
       <c r="F17" s="67"/>
-      <c r="G17" s="66"/>
       <c r="AHE17" s="0"/>
       <c r="AHF17" s="0"/>
       <c r="AHG17" s="0"/>
@@ -8838,6 +8661,7 @@
       <c r="D18" s="65"/>
       <c r="E18" s="65"/>
       <c r="F18" s="67"/>
+      <c r="G18" s="66"/>
       <c r="AHE18" s="0"/>
       <c r="AHF18" s="0"/>
       <c r="AHG18" s="0"/>
@@ -8977,9 +8801,7 @@
     </row>
     <row r="19" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="66"/>
+      <c r="E19" s="66"/>
       <c r="AHE19" s="0"/>
       <c r="AHF19" s="0"/>
       <c r="AHG19" s="0"/>
@@ -9119,7 +8941,7 @@
     </row>
     <row r="20" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="65"/>
-      <c r="E20" s="66"/>
+      <c r="E20" s="65"/>
       <c r="AHE20" s="0"/>
       <c r="AHF20" s="0"/>
       <c r="AHG20" s="0"/>
@@ -9680,6 +9502,9 @@
     <row r="24" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="65"/>
       <c r="AHE24" s="0"/>
       <c r="AHF24" s="0"/>
       <c r="AHG24" s="0"/>
@@ -9820,9 +9645,6 @@
     <row r="25" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="65"/>
       <c r="AHE25" s="0"/>
       <c r="AHF25" s="0"/>
       <c r="AHG25" s="0"/>
@@ -9960,146 +9782,6 @@
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
     </row>
-    <row r="26" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="AHE26" s="0"/>
-      <c r="AHF26" s="0"/>
-      <c r="AHG26" s="0"/>
-      <c r="AHH26" s="0"/>
-      <c r="AHI26" s="0"/>
-      <c r="AHJ26" s="0"/>
-      <c r="AHK26" s="0"/>
-      <c r="AHL26" s="0"/>
-      <c r="AHM26" s="0"/>
-      <c r="AHN26" s="0"/>
-      <c r="AHO26" s="0"/>
-      <c r="AHP26" s="0"/>
-      <c r="AHQ26" s="0"/>
-      <c r="AHR26" s="0"/>
-      <c r="AHS26" s="0"/>
-      <c r="AHT26" s="0"/>
-      <c r="AHU26" s="0"/>
-      <c r="AHV26" s="0"/>
-      <c r="AHW26" s="0"/>
-      <c r="AHX26" s="0"/>
-      <c r="AHY26" s="0"/>
-      <c r="AHZ26" s="0"/>
-      <c r="AIA26" s="0"/>
-      <c r="AIB26" s="0"/>
-      <c r="AIC26" s="0"/>
-      <c r="AID26" s="0"/>
-      <c r="AIE26" s="0"/>
-      <c r="AIF26" s="0"/>
-      <c r="AIG26" s="0"/>
-      <c r="AIH26" s="0"/>
-      <c r="AII26" s="0"/>
-      <c r="AIJ26" s="0"/>
-      <c r="AIK26" s="0"/>
-      <c r="AIL26" s="0"/>
-      <c r="AIM26" s="0"/>
-      <c r="AIN26" s="0"/>
-      <c r="AIO26" s="0"/>
-      <c r="AIP26" s="0"/>
-      <c r="AIQ26" s="0"/>
-      <c r="AIR26" s="0"/>
-      <c r="AIS26" s="0"/>
-      <c r="AIT26" s="0"/>
-      <c r="AIU26" s="0"/>
-      <c r="AIV26" s="0"/>
-      <c r="AIW26" s="0"/>
-      <c r="AIX26" s="0"/>
-      <c r="AIY26" s="0"/>
-      <c r="AIZ26" s="0"/>
-      <c r="AJA26" s="0"/>
-      <c r="AJB26" s="0"/>
-      <c r="AJC26" s="0"/>
-      <c r="AJD26" s="0"/>
-      <c r="AJE26" s="0"/>
-      <c r="AJF26" s="0"/>
-      <c r="AJG26" s="0"/>
-      <c r="AJH26" s="0"/>
-      <c r="AJI26" s="0"/>
-      <c r="AJJ26" s="0"/>
-      <c r="AJK26" s="0"/>
-      <c r="AJL26" s="0"/>
-      <c r="AJM26" s="0"/>
-      <c r="AJN26" s="0"/>
-      <c r="AJO26" s="0"/>
-      <c r="AJP26" s="0"/>
-      <c r="AJQ26" s="0"/>
-      <c r="AJR26" s="0"/>
-      <c r="AJS26" s="0"/>
-      <c r="AJT26" s="0"/>
-      <c r="AJU26" s="0"/>
-      <c r="AJV26" s="0"/>
-      <c r="AJW26" s="0"/>
-      <c r="AJX26" s="0"/>
-      <c r="AJY26" s="0"/>
-      <c r="AJZ26" s="0"/>
-      <c r="AKA26" s="0"/>
-      <c r="AKB26" s="0"/>
-      <c r="AKC26" s="0"/>
-      <c r="AKD26" s="0"/>
-      <c r="AKE26" s="0"/>
-      <c r="AKF26" s="0"/>
-      <c r="AKG26" s="0"/>
-      <c r="AKH26" s="0"/>
-      <c r="AKI26" s="0"/>
-      <c r="AKJ26" s="0"/>
-      <c r="AKK26" s="0"/>
-      <c r="AKL26" s="0"/>
-      <c r="AKM26" s="0"/>
-      <c r="AKN26" s="0"/>
-      <c r="AKO26" s="0"/>
-      <c r="AKP26" s="0"/>
-      <c r="AKQ26" s="0"/>
-      <c r="AKR26" s="0"/>
-      <c r="AKS26" s="0"/>
-      <c r="AKT26" s="0"/>
-      <c r="AKU26" s="0"/>
-      <c r="AKV26" s="0"/>
-      <c r="AKW26" s="0"/>
-      <c r="AKX26" s="0"/>
-      <c r="AKY26" s="0"/>
-      <c r="AKZ26" s="0"/>
-      <c r="ALA26" s="0"/>
-      <c r="ALB26" s="0"/>
-      <c r="ALC26" s="0"/>
-      <c r="ALD26" s="0"/>
-      <c r="ALE26" s="0"/>
-      <c r="ALF26" s="0"/>
-      <c r="ALG26" s="0"/>
-      <c r="ALH26" s="0"/>
-      <c r="ALI26" s="0"/>
-      <c r="ALJ26" s="0"/>
-      <c r="ALK26" s="0"/>
-      <c r="ALL26" s="0"/>
-      <c r="ALM26" s="0"/>
-      <c r="ALN26" s="0"/>
-      <c r="ALO26" s="0"/>
-      <c r="ALP26" s="0"/>
-      <c r="ALQ26" s="0"/>
-      <c r="ALR26" s="0"/>
-      <c r="ALS26" s="0"/>
-      <c r="ALT26" s="0"/>
-      <c r="ALU26" s="0"/>
-      <c r="ALV26" s="0"/>
-      <c r="ALW26" s="0"/>
-      <c r="ALX26" s="0"/>
-      <c r="ALY26" s="0"/>
-      <c r="ALZ26" s="0"/>
-      <c r="AMA26" s="0"/>
-      <c r="AMB26" s="0"/>
-      <c r="AMC26" s="0"/>
-      <c r="AMD26" s="0"/>
-      <c r="AME26" s="0"/>
-      <c r="AMF26" s="0"/>
-      <c r="AMG26" s="0"/>
-      <c r="AMH26" s="0"/>
-      <c r="AMI26" s="0"/>
-      <c r="AMJ26" s="0"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
@@ -10118,7 +9800,7 @@
   </sheetPr>
   <dimension ref="A1:IU18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -10145,7 +9827,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10176,10 +9858,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>59</v>
@@ -10188,16 +9870,16 @@
         <v>60</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>61</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>33</v>
@@ -10209,10 +9891,10 @@
         <v>63</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O2" s="69" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P2" s="70"/>
       <c r="Q2" s="47"/>
@@ -10229,7 +9911,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>66</v>
@@ -10238,10 +9920,10 @@
         <v>67</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>68</v>
@@ -10262,7 +9944,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="72" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P3" s="73"/>
       <c r="Q3" s="61"/>
@@ -10274,17 +9956,17 @@
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H4" s="62"/>
       <c r="I4" s="74"/>
@@ -10303,22 +9985,22 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="52" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="51" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K5" s="51" t="s">
         <v>41</v>
@@ -10574,22 +10256,22 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="52" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H6" s="62"/>
       <c r="I6" s="62"/>
       <c r="J6" s="52" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K6" s="51" t="s">
         <v>41</v>
@@ -10945,7 +10627,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10967,16 +10649,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>128</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -10994,10 +10676,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F3" s="76" t="s">
         <v>50</v>
@@ -11016,10 +10698,10 @@
         <v>71</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E4" s="77" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F4" s="62" t="n">
         <v>1</v>
@@ -11034,10 +10716,10 @@
         <v>71</v>
       </c>
       <c r="D5" s="77" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F5" s="62" t="n">
         <v>2</v>
@@ -11093,7 +10775,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -11132,55 +10814,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="T2" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P2" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="R2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11206,43 +10888,43 @@
         <v>50</v>
       </c>
       <c r="H3" s="79" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I3" s="79" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K3" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="R3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="S3" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="T3" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="U3" s="76" t="s">
         <v>153</v>
-      </c>
-      <c r="S3" s="76" t="s">
-        <v>154</v>
-      </c>
-      <c r="T3" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="U3" s="76" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11254,13 +10936,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G4" s="50" t="n">
         <v>1</v>
@@ -11280,7 +10962,7 @@
       <c r="P4" s="50"/>
       <c r="R4" s="50"/>
       <c r="S4" s="80" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T4" s="50"/>
       <c r="U4" s="50"/>
@@ -11294,13 +10976,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G5" s="50" t="n">
         <v>2</v>
@@ -11322,7 +11004,7 @@
       <c r="P5" s="50"/>
       <c r="R5" s="50"/>
       <c r="S5" s="80" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
@@ -11336,13 +11018,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G6" s="50" t="n">
         <v>3</v>
@@ -11364,7 +11046,7 @@
       <c r="P6" s="50"/>
       <c r="R6" s="50"/>
       <c r="S6" s="80" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T6" s="50"/>
       <c r="U6" s="50"/>
@@ -11378,13 +11060,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G7" s="50" t="n">
         <v>4</v>
@@ -11408,7 +11090,7 @@
       <c r="P7" s="50"/>
       <c r="R7" s="50"/>
       <c r="S7" s="80" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
@@ -11429,10 +11111,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG38"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11460,7 +11142,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -11499,55 +11181,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="J2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" s="16" t="s">
+      <c r="N2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="O2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="P2" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="Q2" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="P2" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>184</v>
-      </c>
       <c r="S2" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
@@ -11574,55 +11256,55 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="H3" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="I3" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="J3" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="L3" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="M3" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="22" t="s">
+      <c r="N3" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="O3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="Q3" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="O3" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" s="82" t="s">
+      <c r="S3" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="T3" s="21" t="s">
         <v>196</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11634,7 +11316,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>71</v>
@@ -11645,11 +11327,11 @@
         <v>1</v>
       </c>
       <c r="I4" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J4" s="62"/>
       <c r="K4" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L4" s="51"/>
       <c r="M4" s="62" t="n">
@@ -11672,7 +11354,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>75</v>
@@ -11683,11 +11365,11 @@
         <v>1</v>
       </c>
       <c r="I5" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L5" s="51"/>
       <c r="M5" s="62" t="n">
@@ -11696,7 +11378,7 @@
       <c r="N5" s="62"/>
       <c r="O5" s="62"/>
       <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
+      <c r="Q5" s="51"/>
       <c r="R5" s="74"/>
       <c r="S5" s="62"/>
       <c r="T5" s="62"/>
@@ -11710,10 +11392,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
@@ -11721,11 +11403,11 @@
         <v>1</v>
       </c>
       <c r="I6" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J6" s="62"/>
       <c r="K6" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L6" s="51"/>
       <c r="M6" s="62" t="n">
@@ -11733,7 +11415,7 @@
       </c>
       <c r="N6" s="62"/>
       <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
+      <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
       <c r="R6" s="74"/>
       <c r="S6" s="62"/>
@@ -11748,7 +11430,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>85</v>
@@ -11759,11 +11441,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="62" t="n">
@@ -11786,10 +11468,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -11797,11 +11479,11 @@
         <v>1</v>
       </c>
       <c r="I8" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L8" s="51"/>
       <c r="M8" s="62" t="n">
@@ -11809,7 +11491,7 @@
       </c>
       <c r="N8" s="62"/>
       <c r="O8" s="62"/>
-      <c r="P8" s="51"/>
+      <c r="P8" s="62"/>
       <c r="Q8" s="51"/>
       <c r="R8" s="74"/>
       <c r="S8" s="62"/>
@@ -11824,10 +11506,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -11835,11 +11517,11 @@
         <v>1</v>
       </c>
       <c r="I9" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L9" s="51"/>
       <c r="M9" s="62" t="n">
@@ -11862,10 +11544,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -11873,11 +11555,11 @@
         <v>1</v>
       </c>
       <c r="I10" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J10" s="62"/>
       <c r="K10" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L10" s="51"/>
       <c r="M10" s="62" t="n">
@@ -11900,10 +11582,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -11911,11 +11593,11 @@
         <v>1</v>
       </c>
       <c r="I11" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L11" s="51"/>
       <c r="M11" s="62" t="n">
@@ -11938,10 +11620,10 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -11949,11 +11631,11 @@
         <v>1</v>
       </c>
       <c r="I12" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J12" s="62"/>
       <c r="K12" s="74" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L12" s="51"/>
       <c r="M12" s="62" t="n">
@@ -11975,27 +11657,27 @@
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>157</v>
+      <c r="D13" s="51" t="s">
+        <v>158</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
+        <v>71</v>
+      </c>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
       <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J13" s="62"/>
       <c r="K13" s="74" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L13" s="51"/>
       <c r="M13" s="62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="62"/>
       <c r="O13" s="62"/>
@@ -12014,22 +11696,22 @@
         <v>38</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
+        <v>75</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="74" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J14" s="62"/>
       <c r="K14" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L14" s="51"/>
       <c r="M14" s="62" t="n">
@@ -12037,7 +11719,7 @@
       </c>
       <c r="N14" s="62"/>
       <c r="O14" s="62"/>
-      <c r="P14" s="62"/>
+      <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
       <c r="R14" s="74"/>
       <c r="S14" s="62"/>
@@ -12052,10 +11734,10 @@
         <v>38</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -12063,11 +11745,11 @@
         <v>1</v>
       </c>
       <c r="I15" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J15" s="62"/>
       <c r="K15" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L15" s="51"/>
       <c r="M15" s="62" t="n">
@@ -12090,10 +11772,10 @@
         <v>38</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -12101,11 +11783,11 @@
         <v>1</v>
       </c>
       <c r="I16" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J16" s="62"/>
       <c r="K16" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L16" s="51"/>
       <c r="M16" s="62" t="n">
@@ -12113,7 +11795,7 @@
       </c>
       <c r="N16" s="62"/>
       <c r="O16" s="62"/>
-      <c r="P16" s="51"/>
+      <c r="P16" s="62"/>
       <c r="Q16" s="51"/>
       <c r="R16" s="74"/>
       <c r="S16" s="62"/>
@@ -12128,10 +11810,10 @@
         <v>38</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -12139,11 +11821,11 @@
         <v>1</v>
       </c>
       <c r="I17" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J17" s="62"/>
       <c r="K17" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L17" s="51"/>
       <c r="M17" s="62" t="n">
@@ -12166,10 +11848,10 @@
         <v>38</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -12177,11 +11859,11 @@
         <v>1</v>
       </c>
       <c r="I18" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L18" s="51"/>
       <c r="M18" s="62" t="n">
@@ -12204,10 +11886,10 @@
         <v>38</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -12215,11 +11897,11 @@
         <v>1</v>
       </c>
       <c r="I19" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J19" s="62"/>
       <c r="K19" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L19" s="51"/>
       <c r="M19" s="62" t="n">
@@ -12242,10 +11924,10 @@
         <v>38</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -12253,11 +11935,11 @@
         <v>1</v>
       </c>
       <c r="I20" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J20" s="62"/>
       <c r="K20" s="74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L20" s="51"/>
       <c r="M20" s="62" t="n">
@@ -12280,10 +11962,10 @@
         <v>38</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -12291,11 +11973,11 @@
         <v>1</v>
       </c>
       <c r="I21" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J21" s="62"/>
       <c r="K21" s="74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L21" s="51"/>
       <c r="M21" s="62" t="n">
@@ -12317,11 +11999,11 @@
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="52" t="s">
         <v>161</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -12329,15 +12011,15 @@
         <v>1</v>
       </c>
       <c r="I22" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J22" s="62"/>
       <c r="K22" s="74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L22" s="51"/>
       <c r="M22" s="62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22" s="62"/>
       <c r="O22" s="62"/>
@@ -12355,27 +12037,27 @@
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>96</v>
+      <c r="D23" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>97</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
       <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="83" t="s">
-        <v>200</v>
+      <c r="I23" s="85" t="s">
+        <v>201</v>
       </c>
       <c r="J23" s="62"/>
-      <c r="K23" s="74" t="s">
-        <v>203</v>
+      <c r="K23" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="L23" s="51"/>
       <c r="M23" s="62" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N23" s="62"/>
       <c r="O23" s="62"/>
@@ -12385,81 +12067,29 @@
       <c r="S23" s="62"/>
       <c r="T23" s="62"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="83" t="s">
-        <v>200</v>
-      </c>
-      <c r="J24" s="62"/>
-      <c r="K24" s="74" t="s">
-        <v>203</v>
-      </c>
-      <c r="L24" s="51"/>
-      <c r="M24" s="62" t="n">
-        <v>3</v>
-      </c>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="74"/>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="n">
-        <v>44197</v>
-      </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="62" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="85" t="s">
-        <v>204</v>
-      </c>
-      <c r="J25" s="62"/>
-      <c r="K25" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="L25" s="51"/>
-      <c r="M25" s="62" t="n">
-        <v>4</v>
-      </c>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="Q24" s="87"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="Q25" s="87"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="86"/>
@@ -12519,6 +12149,8 @@
       <c r="G30" s="87"/>
       <c r="K30" s="87"/>
       <c r="L30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="87"/>
       <c r="Q30" s="87"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12526,9 +12158,6 @@
       <c r="B31" s="86"/>
       <c r="C31" s="87"/>
       <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
       <c r="K31" s="87"/>
       <c r="L31" s="87"/>
       <c r="Q31" s="87"/>
@@ -12538,13 +12167,8 @@
       <c r="B32" s="86"/>
       <c r="C32" s="87"/>
       <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
       <c r="K32" s="87"/>
       <c r="L32" s="87"/>
-      <c r="O32" s="87"/>
-      <c r="P32" s="87"/>
       <c r="Q32" s="87"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12552,6 +12176,9 @@
       <c r="B33" s="86"/>
       <c r="C33" s="87"/>
       <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
       <c r="K33" s="87"/>
       <c r="L33" s="87"/>
       <c r="Q33" s="87"/>
@@ -12561,6 +12188,9 @@
       <c r="B34" s="86"/>
       <c r="C34" s="87"/>
       <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
       <c r="K34" s="87"/>
       <c r="L34" s="87"/>
       <c r="Q34" s="87"/>
@@ -12570,9 +12200,9 @@
       <c r="B35" s="86"/>
       <c r="C35" s="87"/>
       <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
       <c r="K35" s="87"/>
       <c r="L35" s="87"/>
       <c r="Q35" s="87"/>
@@ -12582,36 +12212,12 @@
       <c r="B36" s="86"/>
       <c r="C36" s="87"/>
       <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
       <c r="K36" s="87"/>
       <c r="L36" s="87"/>
       <c r="Q36" s="87"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="88"/>
-      <c r="K37" s="87"/>
-      <c r="L37" s="87"/>
-      <c r="Q37" s="87"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="86"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="88"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="87"/>
-      <c r="Q38" s="87"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add segment download implementation and fix recording sharing
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="303">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t xml:space="preserve">Share case hearing recordings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://172.17.0.1:8080/sharees</t>
   </si>
   <si>
     <t xml:space="preserve">CaseEventToFields</t>
@@ -1038,15 +1041,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1217,6 +1221,13 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1456,7 +1467,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1469,7 +1480,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1798,6 +1809,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1814,6 +1829,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1846,11 +1865,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1866,11 +1885,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1890,7 +1909,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1906,14 +1925,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1922,15 +1937,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1938,7 +1957,51 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1946,70 +2009,26 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2022,7 +2041,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2030,7 +2049,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2110,7 +2129,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2118,11 +2137,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2337,7 +2356,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -2364,31 +2383,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -2405,37 +2424,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="90" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="90" t="s">
+      <c r="D3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="E3" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="89" t="s">
-        <v>208</v>
-      </c>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="H3" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="89" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="89" t="s">
+      <c r="I3" s="91" t="s">
+        <v>211</v>
+      </c>
+      <c r="J3" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="91" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2480,7 +2499,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="12" t="s">
@@ -2511,31 +2530,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2549,28 +2568,28 @@
         <v>49</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>109</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>110</v>
@@ -2587,11 +2606,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" s="92" t="s">
+      <c r="E4" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G4" s="62" t="n">
         <v>1</v>
@@ -2615,11 +2634,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F5" s="92" t="s">
+      <c r="E5" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F5" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G5" s="62" t="n">
         <v>1</v>
@@ -2643,11 +2662,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" s="92" t="s">
+      <c r="E6" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G6" s="62" t="n">
         <v>1</v>
@@ -2671,11 +2690,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F7" s="92" t="s">
+      <c r="E7" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F7" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G7" s="62" t="n">
         <v>1</v>
@@ -2699,11 +2718,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F8" s="92" t="s">
+      <c r="E8" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G8" s="62" t="n">
         <v>1</v>
@@ -2727,11 +2746,11 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="92" t="s">
+      <c r="E9" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F9" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
@@ -2755,10 +2774,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="91" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="92" t="s">
+      <c r="E10" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="94" t="s">
         <v>94</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2775,9 +2794,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="87"/>
+      <c r="H11" s="89"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2805,184 +2824,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="93" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="93" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="93" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="93" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="93" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="93" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="93" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="93" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="93" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="93" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="93" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="95" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="95" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="94" t="s">
-        <v>230</v>
-      </c>
-      <c r="B1" s="95" t="s">
+      <c r="A1" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="101" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2" s="101" t="s">
+      <c r="E2" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="102" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="102" t="s">
+      <c r="F2" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="G2" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="101" t="s">
+      <c r="I2" s="105" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
+      <c r="J2" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="104"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="D3" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="E3" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="106" t="s">
-        <v>236</v>
-      </c>
-      <c r="G3" s="106" t="s">
+      <c r="F3" s="108" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="107" t="s">
+      <c r="G3" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="107" t="s">
+      <c r="H3" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="107" t="s">
-        <v>239</v>
-      </c>
-      <c r="K3" s="107" t="s">
+      <c r="J3" s="109" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="107"/>
-      <c r="M3" s="108"/>
+      <c r="K3" s="109" t="s">
+        <v>241</v>
+      </c>
+      <c r="L3" s="109"/>
+      <c r="M3" s="110"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="109"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="109"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="109"/>
-      <c r="B7" s="109"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="111"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="109"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3023,22 +3042,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B1" s="110" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="114" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3052,25 +3071,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3080,11 +3099,11 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="114" t="s">
-        <v>183</v>
+      <c r="D3" s="116" t="s">
+        <v>184</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>107</v>
@@ -3102,14 +3121,14 @@
         <v>110</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3311,7 +3330,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3339,60 +3358,60 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="116" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="117"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
+      <c r="I2" s="118" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="119"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="119" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="90" t="s">
+      <c r="D3" s="121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="121"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="I3" s="122" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="123"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3504,7 +3523,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="123" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="125" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3527,26 +3546,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="86"/>
+      <c r="A10" s="88"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="124"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="124"/>
+      <c r="G11" s="126"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86"/>
-      <c r="G12" s="124"/>
+      <c r="A12" s="88"/>
+      <c r="G12" s="126"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="86"/>
-      <c r="G13" s="124"/>
+      <c r="A13" s="88"/>
+      <c r="G13" s="126"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="G14" s="124"/>
+      <c r="A14" s="88"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3586,8 +3605,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="125" t="s">
-        <v>250</v>
+      <c r="A1" s="127" t="s">
+        <v>251</v>
       </c>
       <c r="B1" s="58" t="s">
         <v>8</v>
@@ -3595,61 +3614,61 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="127" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="127" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="127" t="s">
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="129" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="D2" s="129" t="s">
+        <v>247</v>
+      </c>
+      <c r="E2" s="129" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
+      <c r="F2" s="90" t="s">
+        <v>254</v>
+      </c>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="129" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="128" t="s">
+      <c r="D3" s="131" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="128" t="s">
-        <v>254</v>
-      </c>
-      <c r="I3" s="128" t="s">
+      <c r="H3" s="130" t="s">
         <v>255</v>
+      </c>
+      <c r="I3" s="130" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3677,35 +3696,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="130" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="130" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="130" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="132" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="132" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="130" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="130" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="130" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="132" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="132" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="131" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="132" t="s">
+      <c r="A1" s="133" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="133" t="s">
+      <c r="D1" s="135" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3719,57 +3738,57 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="90" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="90" t="s">
+      <c r="D3" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="89" t="s">
-        <v>221</v>
+      <c r="J3" s="91" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3879,7 +3898,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="135"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3901,7 +3920,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="135"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3917,13 +3936,13 @@
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="135"/>
+      <c r="I10" s="137"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3965,7 +3984,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3993,56 +4012,56 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="119" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="90" t="s">
+      <c r="D3" s="121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="89" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="I3" s="91" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4189,7 +4208,7 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G10" s="74" t="n">
         <v>8</v>
@@ -4199,32 +4218,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="F11" s="136"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
+      <c r="F11" s="138"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="F12" s="136"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="F12" s="138"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="F13" s="136"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="F13" s="138"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="F14" s="136"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="F14" s="138"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4264,7 +4283,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4287,13 +4306,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4304,16 +4323,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4321,10 +4340,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="137" t="s">
-        <v>267</v>
-      </c>
-      <c r="D4" s="137" t="s">
+      <c r="C4" s="139" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="139" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4335,8 +4354,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86"/>
-      <c r="C5" s="138"/>
+      <c r="A5" s="88"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4374,7 +4393,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4396,44 +4415,44 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="139" t="s">
+      <c r="D3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="91" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86"/>
+      <c r="A4" s="88"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86"/>
+      <c r="A5" s="88"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4595,7 +4614,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4616,13 +4635,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4636,25 +4655,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -4671,15 +4690,15 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="53"/>
@@ -4713,7 +4732,7 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -4730,8 +4749,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="140" t="s">
-        <v>278</v>
+      <c r="A1" s="142" t="s">
+        <v>279</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4742,12 +4761,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4757,53 +4776,53 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
+        <v>275</v>
+      </c>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="143" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="143" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="142" t="s">
-        <v>275</v>
-      </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
+      <c r="D3" s="145" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="145" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="144" t="s">
+        <v>276</v>
+      </c>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4811,10 +4830,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -4830,7 +4849,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4838,17 +4857,17 @@
         <v>75</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4856,17 +4875,17 @@
         <v>79</v>
       </c>
       <c r="E6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4874,17 +4893,17 @@
         <v>82</v>
       </c>
       <c r="E7" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="115"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4892,17 +4911,17 @@
         <v>85</v>
       </c>
       <c r="E8" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F8" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="115"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4910,17 +4929,17 @@
         <v>87</v>
       </c>
       <c r="E9" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="115"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4928,17 +4947,17 @@
         <v>89</v>
       </c>
       <c r="E10" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="115"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4946,17 +4965,17 @@
         <v>91</v>
       </c>
       <c r="E11" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="115"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4964,17 +4983,17 @@
         <v>93</v>
       </c>
       <c r="E12" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="115"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -4982,17 +5001,17 @@
         <v>97</v>
       </c>
       <c r="E13" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="115"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -5000,10 +5019,10 @@
         <v>71</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -5019,7 +5038,7 @@
       <c r="A15" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="115"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -5027,17 +5046,17 @@
         <v>75</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="115"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -5045,17 +5064,17 @@
         <v>79</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="115"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -5063,17 +5082,17 @@
         <v>82</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -5081,17 +5100,17 @@
         <v>85</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="115"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -5099,17 +5118,17 @@
         <v>87</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="115"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
@@ -5117,17 +5136,17 @@
         <v>89</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="115"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -5135,17 +5154,17 @@
         <v>91</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="115"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -5153,17 +5172,17 @@
         <v>93</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="115"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -5171,10 +5190,10 @@
         <v>97</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5229,7 +5248,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5251,16 +5270,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -5275,24 +5294,24 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="144" t="s">
-        <v>221</v>
+      <c r="D3" s="146" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="146" t="s">
+        <v>222</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5300,17 +5319,17 @@
         <v>154</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5318,17 +5337,17 @@
         <v>158</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5336,17 +5355,17 @@
         <v>161</v>
       </c>
       <c r="E6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5354,17 +5373,17 @@
         <v>164</v>
       </c>
       <c r="E7" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="115"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -5372,17 +5391,17 @@
         <v>154</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="115"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -5390,17 +5409,17 @@
         <v>158</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="115"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -5408,17 +5427,17 @@
         <v>161</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="115"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -5426,10 +5445,10 @@
         <v>164</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5460,31 +5479,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="145" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="145" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="145" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="145" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="145" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="145" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="145" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="146" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="147" t="s">
+      <c r="A1" s="148" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="148" t="s">
+      <c r="C1" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="149" t="s">
+      <c r="D1" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5494,41 +5513,41 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="151" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="D2" s="153" t="s">
+        <v>285</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
+        <v>275</v>
+      </c>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" s="144" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="153" t="s">
-        <v>275</v>
+      <c r="D3" s="146" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="146" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="155" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5543,10 +5562,10 @@
         <v>52</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -5572,10 +5591,10 @@
         <v>52</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
@@ -5626,7 +5645,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5645,19 +5664,19 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,16 +5690,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>107</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5698,10 +5717,10 @@
         <v>114</v>
       </c>
       <c r="F4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5719,10 +5738,10 @@
         <v>111</v>
       </c>
       <c r="F5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5740,10 +5759,10 @@
         <v>118</v>
       </c>
       <c r="F6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5761,10 +5780,10 @@
         <v>114</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5782,10 +5801,10 @@
         <v>111</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5803,10 +5822,10 @@
         <v>118</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G9" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -5834,68 +5853,68 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="123" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="123" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="123" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="123" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="123" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="125" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="125" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="154" t="s">
-        <v>289</v>
-      </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="156"/>
+      <c r="A1" s="156" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="157" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="157" t="s">
+      <c r="A2" s="159" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="157" t="s">
+      <c r="B2" s="159" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="157" t="s">
+      <c r="C2" s="159" t="s">
         <v>293</v>
       </c>
+      <c r="D2" s="159" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="158" t="s">
-        <v>294</v>
-      </c>
-      <c r="B3" s="158" t="s">
+      <c r="A3" s="160" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="158" t="s">
+      <c r="B3" s="160" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="158" t="s">
+      <c r="C3" s="160" t="s">
         <v>297</v>
       </c>
+      <c r="D3" s="160" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="159" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="160" t="s">
+      <c r="A4" s="161" t="s">
         <v>299</v>
       </c>
-      <c r="C4" s="160" t="s">
+      <c r="B4" s="162" t="s">
         <v>300</v>
       </c>
+      <c r="C4" s="162" t="s">
+        <v>301</v>
+      </c>
       <c r="D4" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="161"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="163"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="165"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6227,7 +6246,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9801,7 +9820,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10744,8 +10763,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10764,7 +10783,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="27.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="28.14"/>
@@ -11086,7 +11105,9 @@
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
+      <c r="O7" s="82" t="s">
+        <v>167</v>
+      </c>
       <c r="P7" s="50"/>
       <c r="R7" s="50"/>
       <c r="S7" s="80" t="s">
@@ -11096,6 +11117,9 @@
       <c r="U7" s="50"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O7" r:id="rId1" display="http://172.17.0.1:8080/sharees"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11113,8 +11137,8 @@
   </sheetPr>
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11132,7 +11156,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="11" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="11" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="11" width="24.71"/>
@@ -11142,7 +11167,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -11181,49 +11206,49 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>136</v>
@@ -11256,55 +11281,55 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="82" t="s">
-        <v>192</v>
+      <c r="P3" s="83" t="s">
+        <v>193</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11326,12 +11351,12 @@
       <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="83" t="s">
-        <v>197</v>
+      <c r="I4" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J4" s="62"/>
       <c r="K4" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L4" s="51"/>
       <c r="M4" s="62" t="n">
@@ -11364,12 +11389,12 @@
       <c r="H5" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="83" t="s">
-        <v>197</v>
+      <c r="I5" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L5" s="51"/>
       <c r="M5" s="62" t="n">
@@ -11402,12 +11427,12 @@
       <c r="H6" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="83" t="s">
-        <v>197</v>
+      <c r="I6" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J6" s="62"/>
       <c r="K6" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L6" s="51"/>
       <c r="M6" s="62" t="n">
@@ -11440,12 +11465,12 @@
       <c r="H7" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="83" t="s">
-        <v>197</v>
+      <c r="I7" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="62" t="n">
@@ -11478,12 +11503,12 @@
       <c r="H8" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="83" t="s">
-        <v>197</v>
+      <c r="I8" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L8" s="51"/>
       <c r="M8" s="62" t="n">
@@ -11516,12 +11541,12 @@
       <c r="H9" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="83" t="s">
-        <v>197</v>
+      <c r="I9" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L9" s="51"/>
       <c r="M9" s="62" t="n">
@@ -11554,12 +11579,12 @@
       <c r="H10" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="83" t="s">
-        <v>197</v>
+      <c r="I10" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J10" s="62"/>
       <c r="K10" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L10" s="51"/>
       <c r="M10" s="62" t="n">
@@ -11592,12 +11617,12 @@
       <c r="H11" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="83" t="s">
-        <v>197</v>
+      <c r="I11" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L11" s="51"/>
       <c r="M11" s="62" t="n">
@@ -11630,12 +11655,12 @@
       <c r="H12" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="83" t="s">
-        <v>197</v>
+      <c r="I12" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J12" s="62"/>
       <c r="K12" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L12" s="51"/>
       <c r="M12" s="62" t="n">
@@ -11663,17 +11688,17 @@
       <c r="E13" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="83" t="s">
-        <v>197</v>
+      <c r="I13" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J13" s="62"/>
       <c r="K13" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L13" s="51"/>
       <c r="M13" s="62" t="n">
@@ -11706,12 +11731,12 @@
       <c r="H14" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="83" t="s">
-        <v>197</v>
+      <c r="I14" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J14" s="62"/>
       <c r="K14" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L14" s="51"/>
       <c r="M14" s="62" t="n">
@@ -11744,12 +11769,12 @@
       <c r="H15" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="83" t="s">
-        <v>197</v>
+      <c r="I15" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J15" s="62"/>
       <c r="K15" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L15" s="51"/>
       <c r="M15" s="62" t="n">
@@ -11782,12 +11807,12 @@
       <c r="H16" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="83" t="s">
-        <v>197</v>
+      <c r="I16" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J16" s="62"/>
       <c r="K16" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L16" s="51"/>
       <c r="M16" s="62" t="n">
@@ -11820,12 +11845,12 @@
       <c r="H17" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="83" t="s">
-        <v>197</v>
+      <c r="I17" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J17" s="62"/>
       <c r="K17" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L17" s="51"/>
       <c r="M17" s="62" t="n">
@@ -11858,12 +11883,12 @@
       <c r="H18" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="83" t="s">
-        <v>197</v>
+      <c r="I18" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L18" s="51"/>
       <c r="M18" s="62" t="n">
@@ -11896,12 +11921,12 @@
       <c r="H19" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="83" t="s">
-        <v>197</v>
+      <c r="I19" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J19" s="62"/>
       <c r="K19" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L19" s="51"/>
       <c r="M19" s="62" t="n">
@@ -11934,12 +11959,12 @@
       <c r="H20" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="83" t="s">
-        <v>197</v>
+      <c r="I20" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J20" s="62"/>
       <c r="K20" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L20" s="51"/>
       <c r="M20" s="62" t="n">
@@ -11972,12 +11997,12 @@
       <c r="H21" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="83" t="s">
-        <v>197</v>
+      <c r="I21" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J21" s="62"/>
       <c r="K21" s="74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L21" s="51"/>
       <c r="M21" s="62" t="n">
@@ -12010,12 +12035,12 @@
       <c r="H22" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="83" t="s">
-        <v>197</v>
+      <c r="I22" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J22" s="62"/>
       <c r="K22" s="74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L22" s="51"/>
       <c r="M22" s="62" t="n">
@@ -12048,12 +12073,12 @@
       <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="85" t="s">
-        <v>201</v>
+      <c r="I23" s="86" t="s">
+        <v>202</v>
       </c>
       <c r="J23" s="62"/>
       <c r="K23" s="25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L23" s="51"/>
       <c r="M23" s="62" t="n">
@@ -12067,157 +12092,183 @@
       <c r="S23" s="62"/>
       <c r="T23" s="62"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="Q24" s="87"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="24" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B24" s="74"/>
+      <c r="C24" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="86" t="s">
+        <v>202</v>
+      </c>
+      <c r="J24" s="62"/>
+      <c r="K24" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="L24" s="51"/>
+      <c r="M24" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="N24" s="62"/>
+      <c r="O24" s="87"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="62"/>
+      <c r="T24" s="62"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="Q25" s="87"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="Q25" s="89"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="86"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="Q26" s="87"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="Q26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="Q27" s="87"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="Q27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="86"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="Q28" s="87"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="Q28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="Q29" s="87"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="Q29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="86"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="87"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="86"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="Q31" s="87"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="Q31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="86"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="Q32" s="87"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="Q32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="86"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="Q33" s="87"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="Q33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="Q34" s="87"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="Q34" s="89"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="Q35" s="87"/>
+      <c r="A35" s="88"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="Q35" s="89"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-      <c r="Q36" s="87"/>
+      <c r="A36" s="88"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="Q36" s="89"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
use caseId and segment to download file
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="302">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -1046,7 +1046,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1218,6 +1218,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1456,7 +1461,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1469,7 +1474,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="167">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1814,6 +1819,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1910,10 +1927,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1922,15 +1935,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1938,7 +1955,51 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1946,70 +2007,26 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2022,7 +2039,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2030,7 +2047,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2110,7 +2127,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2118,11 +2135,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2405,37 +2422,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="93" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="92" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="89" t="s">
+      <c r="K3" s="92" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2587,10 +2604,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2615,10 +2632,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="92" t="s">
+      <c r="F5" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2643,10 +2660,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2671,10 +2688,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="91" t="s">
+      <c r="E7" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2699,10 +2716,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="91" t="s">
+      <c r="E8" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="92" t="s">
+      <c r="F8" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2727,10 +2744,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="91" t="s">
+      <c r="E9" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
@@ -2755,10 +2772,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="91" t="s">
+      <c r="E10" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="92" t="s">
+      <c r="F10" s="95" t="s">
         <v>94</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2775,9 +2792,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
+      <c r="A11" s="89"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="87"/>
+      <c r="H11" s="90"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2805,184 +2822,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="93" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="93" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="93" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="93" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="93" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="93" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="93" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="93" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="93" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="93" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="93" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="96" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="96" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="96" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="96" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="96" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="96" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="97" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="104" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="104" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="102" t="s">
+      <c r="G2" s="105" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="102" t="s">
+      <c r="H2" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="101" t="s">
+      <c r="J2" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="D3" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="E3" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="F3" s="109" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="G3" s="109" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="107" t="s">
+      <c r="H3" s="110" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="107" t="s">
+      <c r="I3" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="J3" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="107"/>
-      <c r="M3" s="108"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="111"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="109"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="109"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="112"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="109"/>
-      <c r="B7" s="109"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="112"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="109"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3025,20 +3042,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="115" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3080,10 +3097,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="117" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3109,7 +3126,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3353,46 +3370,46 @@
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="116" t="s">
+      <c r="I2" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="117"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="120" t="s">
+      <c r="I3" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="121"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3504,7 +3521,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="123" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="126" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3527,26 +3544,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="86"/>
+      <c r="A10" s="89"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="124"/>
+      <c r="G10" s="127"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
+      <c r="A11" s="89"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="124"/>
+      <c r="G11" s="127"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86"/>
-      <c r="G12" s="124"/>
+      <c r="A12" s="89"/>
+      <c r="G12" s="127"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="86"/>
-      <c r="G13" s="124"/>
+      <c r="A13" s="89"/>
+      <c r="G13" s="127"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="G14" s="124"/>
+      <c r="A14" s="89"/>
+      <c r="G14" s="127"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3586,7 +3603,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="128" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3595,60 +3612,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="127" t="s">
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="130" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="130" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="127" t="s">
+      <c r="E2" s="130" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="91" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="132" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="128" t="s">
+      <c r="G3" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="128" t="s">
+      <c r="H3" s="131" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="128" t="s">
+      <c r="I3" s="131" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3677,35 +3694,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="130" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="130" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="130" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="133" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="133" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="130" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="130" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="130" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="133" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="133" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="133" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="134" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="133" t="s">
+      <c r="D1" s="136" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,34 +3758,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="92" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3879,7 +3896,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="135"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3901,7 +3918,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="135"/>
+      <c r="I9" s="138"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3923,7 +3940,7 @@
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="135"/>
+      <c r="I10" s="138"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4012,37 +4029,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="89" t="s">
+      <c r="H3" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="92" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4199,32 +4216,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="F11" s="136"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="F11" s="139"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="F12" s="136"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="F12" s="139"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="F13" s="136"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="F13" s="139"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="F14" s="136"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="139"/>
+      <c r="F14" s="139"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4321,10 +4338,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="137" t="s">
+      <c r="C4" s="140" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="137" t="s">
+      <c r="D4" s="140" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4335,8 +4352,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86"/>
-      <c r="C5" s="138"/>
+      <c r="A5" s="89"/>
+      <c r="C5" s="141"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4409,31 +4426,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="139" t="s">
+      <c r="D3" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="92" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86"/>
+      <c r="A4" s="89"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86"/>
+      <c r="A5" s="89"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4646,7 +4663,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4671,7 +4688,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4713,7 +4730,7 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -4730,7 +4747,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="143" t="s">
         <v>278</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4742,12 +4759,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4768,42 +4785,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="143" t="s">
+      <c r="D3" s="146" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="143" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="142" t="s">
+      <c r="F3" s="145" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4830,7 +4847,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4848,7 +4865,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4866,7 +4883,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4884,7 +4901,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="115"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4902,7 +4919,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="115"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4920,7 +4937,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="115"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4938,7 +4955,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="115"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4956,7 +4973,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="115"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4974,7 +4991,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="115"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -4992,7 +5009,7 @@
       <c r="A14" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="115"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -5019,7 +5036,7 @@
       <c r="A15" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="115"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -5037,7 +5054,7 @@
       <c r="A16" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="115"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -5055,7 +5072,7 @@
       <c r="A17" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="115"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -5073,7 +5090,7 @@
       <c r="A18" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="118"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -5091,7 +5108,7 @@
       <c r="A19" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="115"/>
+      <c r="B19" s="118"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -5109,7 +5126,7 @@
       <c r="A20" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="115"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
@@ -5127,7 +5144,7 @@
       <c r="A21" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="115"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -5145,7 +5162,7 @@
       <c r="A22" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="115"/>
+      <c r="B22" s="118"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -5163,7 +5180,7 @@
       <c r="A23" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="115"/>
+      <c r="B23" s="118"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -5275,13 +5292,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="147" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5292,7 +5309,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="115"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5310,7 +5327,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5328,7 +5345,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5346,7 +5363,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="115"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5364,7 +5381,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="115"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -5382,7 +5399,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="115"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -5400,7 +5417,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="115"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -5418,7 +5435,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="115"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -5460,31 +5477,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="145" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="145" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="145" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="145" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="145" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="145" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="145" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="149" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="148" t="s">
+      <c r="C1" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="149" t="s">
+      <c r="D1" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5496,7 +5513,7 @@
       <c r="C2" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="151" t="s">
+      <c r="D2" s="154" t="s">
         <v>284</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5505,29 +5522,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="147" t="s">
         <v>285</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="147" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="156" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5834,57 +5851,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="123" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="123" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="123" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="123" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="123" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="126" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="126" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="126" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="126" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="126" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="157" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="156"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="159"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="160" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="157" t="s">
+      <c r="B2" s="160" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="157" t="s">
+      <c r="C2" s="160" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="157" t="s">
+      <c r="D2" s="160" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="161" t="s">
         <v>294</v>
       </c>
-      <c r="B3" s="158" t="s">
+      <c r="B3" s="161" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="158" t="s">
+      <c r="C3" s="161" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="158" t="s">
+      <c r="D3" s="161" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="162" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="163" t="s">
         <v>299</v>
       </c>
-      <c r="C4" s="160" t="s">
+      <c r="C4" s="163" t="s">
         <v>300</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -5892,10 +5909,10 @@
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="161"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="163"/>
+      <c r="A5" s="164"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="166"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6227,7 +6244,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9801,7 +9818,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10745,7 +10762,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11113,8 +11130,8 @@
   </sheetPr>
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12067,157 +12084,179 @@
       <c r="S23" s="62"/>
       <c r="T23" s="62"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="Q24" s="87"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="24" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B24" s="74"/>
+      <c r="C24" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="87" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24" s="62"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="62"/>
+      <c r="T24" s="62"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="Q25" s="87"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="Q25" s="90"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="86"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="Q26" s="87"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="Q26" s="90"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="Q27" s="87"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="Q27" s="90"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="86"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="Q28" s="87"/>
+      <c r="A28" s="89"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="Q28" s="90"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="Q29" s="87"/>
+      <c r="A29" s="89"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="Q29" s="90"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="86"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="87"/>
+      <c r="A30" s="89"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="90"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="86"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="Q31" s="87"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="90"/>
+      <c r="Q31" s="90"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="86"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="Q32" s="87"/>
+      <c r="A32" s="89"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="Q32" s="90"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="86"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="Q33" s="87"/>
+      <c r="A33" s="89"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="Q33" s="90"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="K34" s="87"/>
-      <c r="L34" s="87"/>
-      <c r="Q34" s="87"/>
+      <c r="A34" s="89"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="Q34" s="90"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="Q35" s="87"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="Q35" s="90"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="87"/>
-      <c r="Q36" s="87"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91"/>
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="Q36" s="90"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
revert to using recordingId as caseId is not set yet
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="302">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -1474,7 +1474,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="165">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1816,14 +1816,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2422,37 +2414,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="90" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2604,10 +2596,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2632,10 +2624,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2660,10 +2652,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="94" t="s">
+      <c r="E6" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2688,10 +2680,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2716,10 +2708,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="94" t="s">
+      <c r="E8" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2744,10 +2736,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
@@ -2772,10 +2764,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="93" t="s">
         <v>94</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2792,9 +2784,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
+      <c r="A11" s="87"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="90"/>
+      <c r="H11" s="88"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2822,184 +2814,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="96" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="96" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="96" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="96" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="96" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="96" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="94" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="94" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="94" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="94" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="94" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="94" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="94" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="94" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="94" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="102" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="102" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="103" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="102" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="105"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="107" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="109" t="s">
+      <c r="G3" s="107" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="110" t="s">
+      <c r="H3" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="110" t="s">
+      <c r="I3" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="110" t="s">
+      <c r="J3" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="110" t="s">
+      <c r="K3" s="108" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="110"/>
-      <c r="M3" s="111"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="112"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
+      <c r="A5" s="110"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="112"/>
-      <c r="B6" s="112"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="110"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="112"/>
-      <c r="B7" s="112"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="110"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="112"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="99"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3042,20 +3034,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="113" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3097,10 +3089,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="115" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3126,7 +3118,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3370,46 +3362,46 @@
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="119" t="s">
+      <c r="I2" s="117" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="120"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="123" t="s">
+      <c r="I3" s="121" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="124"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3521,7 +3513,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="126" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="124" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3544,26 +3536,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="89"/>
+      <c r="A10" s="87"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="127"/>
+      <c r="G10" s="125"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
+      <c r="A11" s="87"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="127"/>
+      <c r="G11" s="125"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="89"/>
-      <c r="G12" s="127"/>
+      <c r="A12" s="87"/>
+      <c r="G12" s="125"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89"/>
-      <c r="G13" s="127"/>
+      <c r="A13" s="87"/>
+      <c r="G13" s="125"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89"/>
-      <c r="G14" s="127"/>
+      <c r="A14" s="87"/>
+      <c r="G14" s="125"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3603,7 +3595,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="126" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3612,60 +3604,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="129" t="s">
+      <c r="D1" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="130" t="s">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="C3" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="130" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="131" t="s">
+      <c r="E3" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="131" t="s">
+      <c r="F3" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="131" t="s">
+      <c r="G3" s="129" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="129" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="131" t="s">
+      <c r="I3" s="129" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3694,35 +3686,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="133" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="133" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="131" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="131" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="131" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="133" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="133" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="133" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="131" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="131" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="131" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="132" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="134" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3758,34 +3750,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="90" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3896,7 +3888,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="138"/>
+      <c r="I8" s="136"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3918,7 +3910,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="138"/>
+      <c r="I9" s="136"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3940,7 +3932,7 @@
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="138"/>
+      <c r="I10" s="136"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4029,37 +4021,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4216,32 +4208,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="139"/>
-      <c r="F11" s="139"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="137"/>
+      <c r="F11" s="137"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="F12" s="139"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="F12" s="137"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="F13" s="139"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="F13" s="137"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="139"/>
-      <c r="D14" s="139"/>
-      <c r="F14" s="139"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="F14" s="137"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4338,10 +4330,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="138" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="138" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4352,8 +4344,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89"/>
-      <c r="C5" s="141"/>
+      <c r="A5" s="87"/>
+      <c r="C5" s="139"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4426,31 +4418,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="D3" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="90" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89"/>
+      <c r="A4" s="87"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89"/>
+      <c r="A5" s="87"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4663,7 +4655,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4688,7 +4680,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4747,7 +4739,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="141" t="s">
         <v>278</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4759,12 +4751,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4785,42 +4777,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="144" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="144" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="145" t="s">
+      <c r="F3" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4847,7 +4839,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4865,7 +4857,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4883,7 +4875,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4901,7 +4893,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="118"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4919,7 +4911,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="118"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4937,7 +4929,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="118"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4955,7 +4947,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4973,7 +4965,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="118"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4991,7 +4983,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="118"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -5009,7 +5001,7 @@
       <c r="A14" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="118"/>
+      <c r="B14" s="116"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -5036,7 +5028,7 @@
       <c r="A15" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="118"/>
+      <c r="B15" s="116"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -5054,7 +5046,7 @@
       <c r="A16" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="118"/>
+      <c r="B16" s="116"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -5072,7 +5064,7 @@
       <c r="A17" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="118"/>
+      <c r="B17" s="116"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -5090,7 +5082,7 @@
       <c r="A18" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="118"/>
+      <c r="B18" s="116"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -5108,7 +5100,7 @@
       <c r="A19" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="118"/>
+      <c r="B19" s="116"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -5126,7 +5118,7 @@
       <c r="A20" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="118"/>
+      <c r="B20" s="116"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
@@ -5144,7 +5136,7 @@
       <c r="A21" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="118"/>
+      <c r="B21" s="116"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -5162,7 +5154,7 @@
       <c r="A22" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="118"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -5180,7 +5172,7 @@
       <c r="A23" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="118"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -5292,13 +5284,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5309,7 +5301,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5327,7 +5319,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5345,7 +5337,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5363,7 +5355,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5381,7 +5373,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="118"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -5399,7 +5391,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="118"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -5417,7 +5409,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="118"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -5435,7 +5427,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -5477,31 +5469,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="146" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="146" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="146" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="146" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="146" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="146" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="147" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="152" t="s">
+      <c r="D1" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5513,7 +5505,7 @@
       <c r="C2" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="152" t="s">
         <v>284</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5522,29 +5514,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="145" t="s">
         <v>285</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="154" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5851,57 +5843,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="126" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="126" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="126" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="126" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="126" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="124" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="124" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="155" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="157"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="158" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="158" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="158" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="158" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="159" t="s">
         <v>294</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="159" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="159" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="161" t="s">
+      <c r="D3" s="159" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="162" t="s">
+      <c r="A4" s="160" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="161" t="s">
         <v>299</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="161" t="s">
         <v>300</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -5909,10 +5901,10 @@
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="164"/>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="166"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="164"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11130,8 +11122,8 @@
   </sheetPr>
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12092,7 +12084,7 @@
       <c r="C24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="D24" s="51" t="s">
         <v>164</v>
       </c>
       <c r="E24" s="52" t="s">
@@ -12103,13 +12095,17 @@
       <c r="H24" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="87" t="s">
+      <c r="I24" s="85" t="s">
         <v>201</v>
       </c>
       <c r="J24" s="62"/>
-      <c r="K24" s="88"/>
+      <c r="K24" s="86" t="s">
+        <v>202</v>
+      </c>
       <c r="L24" s="51"/>
-      <c r="M24" s="62"/>
+      <c r="M24" s="62" t="n">
+        <v>4</v>
+      </c>
       <c r="N24" s="62"/>
       <c r="O24" s="62"/>
       <c r="P24" s="62"/>
@@ -12119,144 +12115,144 @@
       <c r="T24" s="62"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="Q25" s="90"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="Q25" s="88"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="Q26" s="90"/>
+      <c r="A26" s="87"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="Q26" s="88"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="Q27" s="90"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="Q27" s="88"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="Q28" s="90"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="Q28" s="88"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="Q29" s="90"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="Q29" s="88"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="90"/>
-      <c r="Q30" s="90"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="88"/>
+      <c r="Q30" s="88"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="Q31" s="90"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="Q31" s="88"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="Q32" s="90"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="Q32" s="88"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="Q33" s="90"/>
+      <c r="A33" s="87"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="Q33" s="88"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="89"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="90"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="90"/>
-      <c r="G34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="Q34" s="90"/>
+      <c r="A34" s="87"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
+      <c r="G34" s="88"/>
+      <c r="K34" s="88"/>
+      <c r="L34" s="88"/>
+      <c r="Q34" s="88"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="89"/>
-      <c r="B35" s="89"/>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="91"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="Q35" s="90"/>
+      <c r="A35" s="87"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="Q35" s="88"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="89"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="K36" s="90"/>
-      <c r="L36" s="90"/>
-      <c r="Q36" s="90"/>
+      <c r="A36" s="87"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="Q36" s="88"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
guard against null recording-time
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -1038,13 +1038,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1819,7 +1820,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1855,11 +1856,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1875,11 +1876,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1899,7 +1900,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1915,7 +1916,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6236,7 +6237,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11122,8 +11123,8 @@
   </sheetPr>
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11141,7 +11142,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="11" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="29.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="11" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="11" width="24.71"/>
@@ -12099,7 +12101,7 @@
         <v>201</v>
       </c>
       <c r="J24" s="62"/>
-      <c r="K24" s="86" t="s">
+      <c r="K24" s="74" t="s">
         <v>202</v>
       </c>
       <c r="L24" s="51"/>
@@ -12107,7 +12109,7 @@
         <v>4</v>
       </c>
       <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
+      <c r="O24" s="86"/>
       <c r="P24" s="62"/>
       <c r="Q24" s="51"/>
       <c r="R24" s="74"/>

</xml_diff>

<commit_message>
tidy up share and download code
</commit_message>
<xml_diff>
--- a/src/aat/resources/CCD_CVP_v.03.xlsx
+++ b/src/aat/resources/CCD_CVP_v.03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="303">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t xml:space="preserve">Share case hearing recordings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://172.17.0.1:8080/sharees</t>
   </si>
   <si>
     <t xml:space="preserve">CaseEventToFields</t>
@@ -1222,8 +1225,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1475,7 +1480,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1804,6 +1809,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1820,7 +1829,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2347,7 +2356,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -2374,31 +2383,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -2415,37 +2424,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="91" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="91" t="s">
+      <c r="D3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="E3" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="90" t="s">
-        <v>208</v>
-      </c>
-      <c r="H3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="90" t="s">
+      <c r="I3" s="91" t="s">
+        <v>211</v>
+      </c>
+      <c r="J3" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="91" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2490,7 +2499,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="12" t="s">
@@ -2521,31 +2530,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2559,28 +2568,28 @@
         <v>49</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>109</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>110</v>
@@ -2597,11 +2606,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" s="93" t="s">
+      <c r="E4" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G4" s="62" t="n">
         <v>1</v>
@@ -2625,11 +2634,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F5" s="93" t="s">
+      <c r="E5" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F5" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G5" s="62" t="n">
         <v>1</v>
@@ -2653,11 +2662,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G6" s="62" t="n">
         <v>1</v>
@@ -2681,11 +2690,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F7" s="93" t="s">
+      <c r="E7" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F7" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G7" s="62" t="n">
         <v>1</v>
@@ -2709,11 +2718,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F8" s="93" t="s">
+      <c r="E8" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G8" s="62" t="n">
         <v>1</v>
@@ -2737,11 +2746,11 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="93" t="s">
+      <c r="E9" s="93" t="s">
         <v>228</v>
+      </c>
+      <c r="F9" s="94" t="s">
+        <v>229</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
@@ -2765,10 +2774,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="92" t="s">
-        <v>229</v>
-      </c>
-      <c r="F10" s="93" t="s">
+      <c r="E10" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="94" t="s">
         <v>94</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2785,9 +2794,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="88"/>
+      <c r="H11" s="89"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2815,184 +2824,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="94" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="94" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="94" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="94" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="94" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="94" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="94" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="94" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="94" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="95" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="95" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="95" t="s">
-        <v>230</v>
-      </c>
-      <c r="B1" s="96" t="s">
+      <c r="A1" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="102" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2" s="102" t="s">
+      <c r="E2" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="103" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="103" t="s">
+      <c r="F2" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="G2" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="102" t="s">
+      <c r="I2" s="105" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
+      <c r="J2" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="104"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="107" t="s">
-        <v>236</v>
-      </c>
-      <c r="G3" s="107" t="s">
+      <c r="F3" s="108" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="G3" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="H3" s="109" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="108" t="s">
-        <v>239</v>
-      </c>
-      <c r="K3" s="108" t="s">
+      <c r="J3" s="109" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="109"/>
+      <c r="K3" s="109" t="s">
+        <v>241</v>
+      </c>
+      <c r="L3" s="109"/>
+      <c r="M3" s="110"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="111"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3033,22 +3042,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B1" s="111" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="114" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3062,25 +3071,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3090,11 +3099,11 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="115" t="s">
-        <v>183</v>
+      <c r="D3" s="116" t="s">
+        <v>184</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>107</v>
@@ -3112,14 +3121,14 @@
         <v>110</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3321,7 +3330,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3349,60 +3358,60 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="117" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="I2" s="118" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="119"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="91" t="s">
+      <c r="D3" s="121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="121" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="122"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="I3" s="122" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="123"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3514,7 +3523,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="124" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="125" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3537,26 +3546,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="87"/>
+      <c r="A10" s="88"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="125"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="125"/>
+      <c r="G11" s="126"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="G12" s="125"/>
+      <c r="A12" s="88"/>
+      <c r="G12" s="126"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="G13" s="125"/>
+      <c r="A13" s="88"/>
+      <c r="G13" s="126"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="G14" s="125"/>
+      <c r="A14" s="88"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3596,8 +3605,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="126" t="s">
-        <v>250</v>
+      <c r="A1" s="127" t="s">
+        <v>251</v>
       </c>
       <c r="B1" s="58" t="s">
         <v>8</v>
@@ -3605,61 +3614,61 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="128" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="128" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="128" t="s">
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="129" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="D2" s="129" t="s">
+        <v>247</v>
+      </c>
+      <c r="E2" s="129" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
+      <c r="F2" s="90" t="s">
+        <v>254</v>
+      </c>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="130" t="s">
+      <c r="C3" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="130" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="129" t="s">
+      <c r="D3" s="131" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="129" t="s">
-        <v>254</v>
-      </c>
-      <c r="I3" s="129" t="s">
+      <c r="H3" s="130" t="s">
         <v>255</v>
+      </c>
+      <c r="I3" s="130" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3687,35 +3696,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="131" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="131" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="132" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="132" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="131" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="131" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="132" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="132" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="132" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="133" t="s">
+      <c r="A1" s="133" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="135" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3729,57 +3738,57 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="91" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="91" t="s">
+      <c r="D3" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="90" t="s">
-        <v>221</v>
+      <c r="J3" s="91" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3889,7 +3898,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="136"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3911,7 +3920,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="136"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3927,13 +3936,13 @@
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="136"/>
+      <c r="I10" s="137"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3975,7 +3984,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4003,56 +4012,56 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="91" t="s">
+      <c r="D3" s="121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="90" t="s">
-        <v>221</v>
-      </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="I3" s="91" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4199,7 +4208,7 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G10" s="74" t="n">
         <v>8</v>
@@ -4209,32 +4218,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="F11" s="137"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
+      <c r="F11" s="138"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="F12" s="137"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="F12" s="138"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
-      <c r="F13" s="137"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="F13" s="138"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="F14" s="137"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="F14" s="138"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4274,7 +4283,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4297,13 +4306,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4314,16 +4323,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4331,10 +4340,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="138" t="s">
-        <v>267</v>
-      </c>
-      <c r="D4" s="138" t="s">
+      <c r="C4" s="139" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="139" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4345,8 +4354,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
-      <c r="C5" s="139"/>
+      <c r="A5" s="88"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4384,7 +4393,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4406,44 +4415,44 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="140" t="s">
+      <c r="D3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="87"/>
+      <c r="A4" s="88"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
+      <c r="A5" s="88"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4605,7 +4614,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4626,13 +4635,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4646,25 +4655,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -4681,15 +4690,15 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="53"/>
@@ -4740,8 +4749,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="141" t="s">
-        <v>278</v>
+      <c r="A1" s="142" t="s">
+        <v>279</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4752,12 +4761,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4767,53 +4776,53 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
+        <v>275</v>
+      </c>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="144" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="143" t="s">
-        <v>275</v>
-      </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="D3" s="145" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="145" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="144" t="s">
+        <v>276</v>
+      </c>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4821,10 +4830,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -4840,7 +4849,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4848,17 +4857,17 @@
         <v>75</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4866,17 +4875,17 @@
         <v>79</v>
       </c>
       <c r="E6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4884,17 +4893,17 @@
         <v>82</v>
       </c>
       <c r="E7" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="116"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4902,17 +4911,17 @@
         <v>85</v>
       </c>
       <c r="E8" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F8" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="116"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4920,17 +4929,17 @@
         <v>87</v>
       </c>
       <c r="E9" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="116"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4938,17 +4947,17 @@
         <v>89</v>
       </c>
       <c r="E10" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4956,17 +4965,17 @@
         <v>91</v>
       </c>
       <c r="E11" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="116"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4974,17 +4983,17 @@
         <v>93</v>
       </c>
       <c r="E12" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -4992,17 +5001,17 @@
         <v>97</v>
       </c>
       <c r="E13" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="116"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -5010,10 +5019,10 @@
         <v>71</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -5029,7 +5038,7 @@
       <c r="A15" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="116"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -5037,17 +5046,17 @@
         <v>75</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="116"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -5055,17 +5064,17 @@
         <v>79</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="116"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -5073,17 +5082,17 @@
         <v>82</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="116"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -5091,17 +5100,17 @@
         <v>85</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="116"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -5109,17 +5118,17 @@
         <v>87</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="116"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
@@ -5127,17 +5136,17 @@
         <v>89</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="116"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -5145,17 +5154,17 @@
         <v>91</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="116"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -5163,17 +5172,17 @@
         <v>93</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="116"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -5181,10 +5190,10 @@
         <v>97</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5239,7 +5248,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5261,16 +5270,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -5285,24 +5294,24 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="145" t="s">
-        <v>221</v>
+      <c r="D3" s="146" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="146" t="s">
+        <v>222</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5310,17 +5319,17 @@
         <v>154</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5328,17 +5337,17 @@
         <v>158</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5346,17 +5355,17 @@
         <v>161</v>
       </c>
       <c r="E6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5364,17 +5373,17 @@
         <v>164</v>
       </c>
       <c r="E7" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="116"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -5382,17 +5391,17 @@
         <v>154</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="116"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -5400,17 +5409,17 @@
         <v>158</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="116"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -5418,17 +5427,17 @@
         <v>161</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -5436,10 +5445,10 @@
         <v>164</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5470,31 +5479,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="146" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="146" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="146" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="146" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="146" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="146" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="147" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="148" t="s">
+      <c r="A1" s="148" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="150" t="s">
+      <c r="D1" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5504,41 +5513,41 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="152" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="D2" s="153" t="s">
+        <v>285</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
+        <v>275</v>
+      </c>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" s="145" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="154" t="s">
-        <v>275</v>
+      <c r="D3" s="146" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="146" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="155" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5553,10 +5562,10 @@
         <v>52</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -5582,10 +5591,10 @@
         <v>52</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
@@ -5636,7 +5645,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5655,19 +5664,19 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5681,16 +5690,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E3" s="48" t="s">
         <v>107</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5708,10 +5717,10 @@
         <v>114</v>
       </c>
       <c r="F4" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5729,10 +5738,10 @@
         <v>111</v>
       </c>
       <c r="F5" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G5" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5750,10 +5759,10 @@
         <v>118</v>
       </c>
       <c r="F6" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" s="51" t="s">
         <v>276</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5771,10 +5780,10 @@
         <v>114</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5792,10 +5801,10 @@
         <v>111</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5813,10 +5822,10 @@
         <v>118</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G9" s="51" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -5844,68 +5853,68 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="124" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="124" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="125" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="125" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="155" t="s">
-        <v>289</v>
-      </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="157"/>
+      <c r="A1" s="156" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="158" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="158" t="s">
+      <c r="A2" s="159" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="158" t="s">
+      <c r="B2" s="159" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="158" t="s">
+      <c r="C2" s="159" t="s">
         <v>293</v>
       </c>
+      <c r="D2" s="159" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="159" t="s">
-        <v>294</v>
-      </c>
-      <c r="B3" s="159" t="s">
+      <c r="A3" s="160" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="B3" s="160" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="C3" s="160" t="s">
         <v>297</v>
       </c>
+      <c r="D3" s="160" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="160" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="161" t="s">
+      <c r="A4" s="161" t="s">
         <v>299</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="B4" s="162" t="s">
         <v>300</v>
       </c>
+      <c r="C4" s="162" t="s">
+        <v>301</v>
+      </c>
       <c r="D4" s="25" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="162"/>
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="164"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="165"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10754,8 +10763,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10774,7 +10783,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="27.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="28.14"/>
@@ -11096,7 +11105,9 @@
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
+      <c r="O7" s="82" t="s">
+        <v>167</v>
+      </c>
       <c r="P7" s="50"/>
       <c r="R7" s="50"/>
       <c r="S7" s="80" t="s">
@@ -11106,6 +11117,9 @@
       <c r="U7" s="50"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O7" r:id="rId1" display="http://172.17.0.1:8080/sharees"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11123,8 +11137,8 @@
   </sheetPr>
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11153,7 +11167,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -11192,49 +11206,49 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J2" s="16" t="s">
         <v>106</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>136</v>
@@ -11267,55 +11281,55 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>110</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O3" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="82" t="s">
-        <v>192</v>
+      <c r="P3" s="83" t="s">
+        <v>193</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11337,12 +11351,12 @@
       <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="83" t="s">
-        <v>197</v>
+      <c r="I4" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J4" s="62"/>
       <c r="K4" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L4" s="51"/>
       <c r="M4" s="62" t="n">
@@ -11375,12 +11389,12 @@
       <c r="H5" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="83" t="s">
-        <v>197</v>
+      <c r="I5" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L5" s="51"/>
       <c r="M5" s="62" t="n">
@@ -11413,12 +11427,12 @@
       <c r="H6" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="83" t="s">
-        <v>197</v>
+      <c r="I6" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J6" s="62"/>
       <c r="K6" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L6" s="51"/>
       <c r="M6" s="62" t="n">
@@ -11451,12 +11465,12 @@
       <c r="H7" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="83" t="s">
-        <v>197</v>
+      <c r="I7" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="62" t="n">
@@ -11489,12 +11503,12 @@
       <c r="H8" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="83" t="s">
-        <v>197</v>
+      <c r="I8" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L8" s="51"/>
       <c r="M8" s="62" t="n">
@@ -11527,12 +11541,12 @@
       <c r="H9" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="83" t="s">
-        <v>197</v>
+      <c r="I9" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L9" s="51"/>
       <c r="M9" s="62" t="n">
@@ -11565,12 +11579,12 @@
       <c r="H10" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="83" t="s">
-        <v>197</v>
+      <c r="I10" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J10" s="62"/>
       <c r="K10" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L10" s="51"/>
       <c r="M10" s="62" t="n">
@@ -11603,12 +11617,12 @@
       <c r="H11" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="83" t="s">
-        <v>197</v>
+      <c r="I11" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L11" s="51"/>
       <c r="M11" s="62" t="n">
@@ -11641,12 +11655,12 @@
       <c r="H12" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="83" t="s">
-        <v>197</v>
+      <c r="I12" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J12" s="62"/>
       <c r="K12" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L12" s="51"/>
       <c r="M12" s="62" t="n">
@@ -11674,17 +11688,17 @@
       <c r="E13" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="83" t="s">
-        <v>197</v>
+      <c r="I13" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J13" s="62"/>
       <c r="K13" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L13" s="51"/>
       <c r="M13" s="62" t="n">
@@ -11717,12 +11731,12 @@
       <c r="H14" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="83" t="s">
-        <v>197</v>
+      <c r="I14" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J14" s="62"/>
       <c r="K14" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L14" s="51"/>
       <c r="M14" s="62" t="n">
@@ -11755,12 +11769,12 @@
       <c r="H15" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="83" t="s">
-        <v>197</v>
+      <c r="I15" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J15" s="62"/>
       <c r="K15" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L15" s="51"/>
       <c r="M15" s="62" t="n">
@@ -11793,12 +11807,12 @@
       <c r="H16" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="83" t="s">
-        <v>197</v>
+      <c r="I16" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J16" s="62"/>
       <c r="K16" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L16" s="51"/>
       <c r="M16" s="62" t="n">
@@ -11831,12 +11845,12 @@
       <c r="H17" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="83" t="s">
-        <v>197</v>
+      <c r="I17" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J17" s="62"/>
       <c r="K17" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L17" s="51"/>
       <c r="M17" s="62" t="n">
@@ -11869,12 +11883,12 @@
       <c r="H18" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="83" t="s">
-        <v>197</v>
+      <c r="I18" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L18" s="51"/>
       <c r="M18" s="62" t="n">
@@ -11907,12 +11921,12 @@
       <c r="H19" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="83" t="s">
-        <v>197</v>
+      <c r="I19" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J19" s="62"/>
       <c r="K19" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L19" s="51"/>
       <c r="M19" s="62" t="n">
@@ -11945,12 +11959,12 @@
       <c r="H20" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="83" t="s">
-        <v>197</v>
+      <c r="I20" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J20" s="62"/>
       <c r="K20" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L20" s="51"/>
       <c r="M20" s="62" t="n">
@@ -11983,12 +11997,12 @@
       <c r="H21" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="83" t="s">
-        <v>197</v>
+      <c r="I21" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J21" s="62"/>
       <c r="K21" s="74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L21" s="51"/>
       <c r="M21" s="62" t="n">
@@ -12021,12 +12035,12 @@
       <c r="H22" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="83" t="s">
-        <v>197</v>
+      <c r="I22" s="84" t="s">
+        <v>198</v>
       </c>
       <c r="J22" s="62"/>
       <c r="K22" s="74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L22" s="51"/>
       <c r="M22" s="62" t="n">
@@ -12059,12 +12073,12 @@
       <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="85" t="s">
-        <v>201</v>
+      <c r="I23" s="86" t="s">
+        <v>202</v>
       </c>
       <c r="J23" s="62"/>
       <c r="K23" s="25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L23" s="51"/>
       <c r="M23" s="62" t="n">
@@ -12097,19 +12111,19 @@
       <c r="H24" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I24" s="85" t="s">
-        <v>201</v>
+      <c r="I24" s="86" t="s">
+        <v>202</v>
       </c>
       <c r="J24" s="62"/>
       <c r="K24" s="74" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L24" s="51"/>
       <c r="M24" s="62" t="n">
         <v>4</v>
       </c>
       <c r="N24" s="62"/>
-      <c r="O24" s="86"/>
+      <c r="O24" s="87"/>
       <c r="P24" s="62"/>
       <c r="Q24" s="51"/>
       <c r="R24" s="74"/>
@@ -12117,144 +12131,144 @@
       <c r="T24" s="62"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="Q25" s="88"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="Q25" s="89"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="Q26" s="88"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="Q26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="87"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="Q27" s="88"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="Q27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="87"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="Q28" s="88"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="Q28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="87"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="Q29" s="88"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="Q29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="87"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="88"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="87"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="Q31" s="88"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="Q31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="87"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="Q32" s="88"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="Q32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="87"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="Q33" s="88"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="Q33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="87"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="Q34" s="88"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="Q34" s="89"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="87"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="Q35" s="88"/>
+      <c r="A35" s="88"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="Q35" s="89"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="87"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="K36" s="88"/>
-      <c r="L36" s="88"/>
-      <c r="Q36" s="88"/>
+      <c r="A36" s="88"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="Q36" s="89"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>